<commit_message>
Code is able to reach level 9 in 22m
</commit_message>
<xml_diff>
--- a/HW2/M2/Regression Formula.xlsx
+++ b/HW2/M2/Regression Formula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\github\side-channels-attacks\HW2\M2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81292EDC-C52E-4873-BD42-66E774DB94BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCECAA80-B4BC-49FA-AA2B-C51561E5F116}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4880" xr2:uid="{1EAE30AF-257F-4C98-8E0D-604CDD161B3C}"/>
   </bookViews>
@@ -24,12 +24,51 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Traces amount needed</t>
+  </si>
+  <si>
+    <r>
+      <t>y = 69.428e</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color rgb="FF595959"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.4582x</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <color rgb="FF595959"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -55,8 +94,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -89,6 +134,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Early Stop</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -161,16 +237,10 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="0.10332385535141432"/>
-                </c:manualLayout>
-              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -203,10 +273,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$1:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -219,26 +289,32 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>Sheet1!$B$1:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,6 +521,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Traces amount needed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -476,7 +577,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.2444444444444437E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.86625240594925634"/>
+          <c:h val="0.72385061242344706"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -517,10 +628,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.3527777777777778"/>
+                  <c:y val="-1.4099956255468067E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -569,6 +686,12 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -579,16 +702,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2266,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC42DDA1-C092-48E0-AEA2-EFECA2F646D1}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2287,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2295,7 +2424,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2306,39 +2435,77 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23">
-        <v>300</v>
+        <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24">
-        <v>500</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:B20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>